<commit_message>
Add DateInterval support in XLSX Reader. Support negative durations in XLSX writer.
</commit_message>
<xml_diff>
--- a/tests/resources/xlsx/sheet_with_same_numeric_value_date_formatted_differently.xlsx
+++ b/tests/resources/xlsx/sheet_with_same_numeric_value_date_formatted_differently.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\nc\github\octaved-flow-openspout\tests\resources\xlsx\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C77A8B-5DCA-4E97-A353-A86B5605FD8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19680" yWindow="16400" windowWidth="34120" windowHeight="23580" tabRatio="500"/>
+    <workbookView xWindow="-28920" yWindow="3375" windowWidth="29040" windowHeight="18240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,8 +25,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="17">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="18">
     <numFmt numFmtId="164" formatCode="[$-409]dddd\,\ mmmm\ d\,\ yy"/>
     <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
     <numFmt numFmtId="166" formatCode="[$-409]d\-mmm\-yyyy;@"/>
@@ -38,6 +44,7 @@
     <numFmt numFmtId="178" formatCode="[$-409]mmmmm;@"/>
     <numFmt numFmtId="179" formatCode="[$-409]mmmmm\-yy;@"/>
     <numFmt numFmtId="180" formatCode="m/d/yyyy;@"/>
+    <numFmt numFmtId="182" formatCode="h:mm:ss"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -169,7 +176,6 @@
     <xf numFmtId="22" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="45" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="47" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="46" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -177,60 +183,69 @@
     <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="169" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="170" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="182" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -555,25 +570,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="20.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>42005</v>
       </c>
@@ -605,7 +620,7 @@
         <v>42005</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>42005</v>
       </c>
@@ -637,7 +652,7 @@
         <v>42005</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="21">
         <v>42005</v>
       </c>
@@ -662,33 +677,33 @@
       <c r="H3" s="28">
         <v>42005</v>
       </c>
-      <c r="I3" s="29">
-        <v>42005</v>
-      </c>
-      <c r="J3" s="30">
+      <c r="I3" s="36">
+        <v>42005</v>
+      </c>
+      <c r="J3" s="29">
         <v>42005</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="31">
-        <v>42005</v>
-      </c>
-      <c r="B4" s="32">
-        <v>42005</v>
-      </c>
-      <c r="C4" s="32">
-        <v>42005</v>
-      </c>
-      <c r="D4" s="33">
-        <v>42005</v>
-      </c>
-      <c r="E4" s="34">
-        <v>42005</v>
-      </c>
-      <c r="F4" s="35">
-        <v>42005</v>
-      </c>
-      <c r="G4" s="36">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="30">
+        <v>42005</v>
+      </c>
+      <c r="B4" s="31">
+        <v>42005</v>
+      </c>
+      <c r="C4" s="31">
+        <v>42005</v>
+      </c>
+      <c r="D4" s="32">
+        <v>42005</v>
+      </c>
+      <c r="E4" s="33">
+        <v>42005</v>
+      </c>
+      <c r="F4" s="34">
+        <v>42005</v>
+      </c>
+      <c r="G4" s="35">
         <v>42005</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Reader\XLSX: add support for DateInterval (#188)
</commit_message>
<xml_diff>
--- a/tests/resources/xlsx/sheet_with_same_numeric_value_date_formatted_differently.xlsx
+++ b/tests/resources/xlsx/sheet_with_same_numeric_value_date_formatted_differently.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\nc\github\octaved-flow-openspout\tests\resources\xlsx\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C77A8B-5DCA-4E97-A353-A86B5605FD8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19680" yWindow="16400" windowWidth="34120" windowHeight="23580" tabRatio="500"/>
+    <workbookView xWindow="-28920" yWindow="3375" windowWidth="29040" windowHeight="18240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,8 +25,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="17">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="18">
     <numFmt numFmtId="164" formatCode="[$-409]dddd\,\ mmmm\ d\,\ yy"/>
     <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
     <numFmt numFmtId="166" formatCode="[$-409]d\-mmm\-yyyy;@"/>
@@ -38,6 +44,7 @@
     <numFmt numFmtId="178" formatCode="[$-409]mmmmm;@"/>
     <numFmt numFmtId="179" formatCode="[$-409]mmmmm\-yy;@"/>
     <numFmt numFmtId="180" formatCode="m/d/yyyy;@"/>
+    <numFmt numFmtId="182" formatCode="h:mm:ss"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -169,7 +176,6 @@
     <xf numFmtId="22" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="45" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="47" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="46" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -177,60 +183,69 @@
     <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="169" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="170" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="182" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -555,25 +570,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="20.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>42005</v>
       </c>
@@ -605,7 +620,7 @@
         <v>42005</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>42005</v>
       </c>
@@ -637,7 +652,7 @@
         <v>42005</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="21">
         <v>42005</v>
       </c>
@@ -662,33 +677,33 @@
       <c r="H3" s="28">
         <v>42005</v>
       </c>
-      <c r="I3" s="29">
-        <v>42005</v>
-      </c>
-      <c r="J3" s="30">
+      <c r="I3" s="36">
+        <v>42005</v>
+      </c>
+      <c r="J3" s="29">
         <v>42005</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="31">
-        <v>42005</v>
-      </c>
-      <c r="B4" s="32">
-        <v>42005</v>
-      </c>
-      <c r="C4" s="32">
-        <v>42005</v>
-      </c>
-      <c r="D4" s="33">
-        <v>42005</v>
-      </c>
-      <c r="E4" s="34">
-        <v>42005</v>
-      </c>
-      <c r="F4" s="35">
-        <v>42005</v>
-      </c>
-      <c r="G4" s="36">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="30">
+        <v>42005</v>
+      </c>
+      <c r="B4" s="31">
+        <v>42005</v>
+      </c>
+      <c r="C4" s="31">
+        <v>42005</v>
+      </c>
+      <c r="D4" s="32">
+        <v>42005</v>
+      </c>
+      <c r="E4" s="33">
+        <v>42005</v>
+      </c>
+      <c r="F4" s="34">
+        <v>42005</v>
+      </c>
+      <c r="G4" s="35">
         <v>42005</v>
       </c>
     </row>

</xml_diff>